<commit_message>
Update location tag BCR names
Our thought is that people are more likely to reference BCR's by number
than by their name. So, move the BCR # to the beginning of the tag name
to make it easier to add.
</commit_message>
<xml_diff>
--- a/dataLoad/tags.xlsx
+++ b/dataLoad/tags.xlsx
@@ -376,117 +376,6 @@
     <t>Zacatecas</t>
   </si>
   <si>
-    <t>Aleutian/Bering Sea Islands (BCR 1)</t>
-  </si>
-  <si>
-    <t>Western Alaska (BCR 2)</t>
-  </si>
-  <si>
-    <t>Arctic Plains and Mountains (BCR 3)</t>
-  </si>
-  <si>
-    <t>Northwestern Interior Forest(BCR 4)</t>
-  </si>
-  <si>
-    <t>Northern Pacific Rainforest (BCR 5)</t>
-  </si>
-  <si>
-    <t>Boreal Taiga Plains (BCR 6)</t>
-  </si>
-  <si>
-    <t>Taiga Shield and Hudson Plain (BCR 7)</t>
-  </si>
-  <si>
-    <t>Boreal Softwood Shield (BCR 8)</t>
-  </si>
-  <si>
-    <t>Great Basin (BCR 9)</t>
-  </si>
-  <si>
-    <t>Northern Rockies (BCR 10)</t>
-  </si>
-  <si>
-    <t>Prairie Potholes (BCR 11)</t>
-  </si>
-  <si>
-    <t>Boreal Hardwood Transition (BCR 12)</t>
-  </si>
-  <si>
-    <t>Lower Great Lakes/St.Lawrence Plain (BCR 13)</t>
-  </si>
-  <si>
-    <t>Atlantic Northern Forests (BCR 14)</t>
-  </si>
-  <si>
-    <t>Sierra Nevada (BCR 15)</t>
-  </si>
-  <si>
-    <t>Southern Rockies Colorado Plateau (BCR 16)</t>
-  </si>
-  <si>
-    <t>Badlands and Prairies (BCR 17)</t>
-  </si>
-  <si>
-    <t>Shortgrass Prairie (BCR 18)</t>
-  </si>
-  <si>
-    <t>Central Mixed Grass Prairie (BCR 19)</t>
-  </si>
-  <si>
-    <t>Edwards Plateau (BCR 20)</t>
-  </si>
-  <si>
-    <t>Oaks and Prairies (BCR 21)</t>
-  </si>
-  <si>
-    <t>Eastern Tallgrass Prairie (BCR 22)</t>
-  </si>
-  <si>
-    <t>Prairie Hardwood Transition (BCR 23)</t>
-  </si>
-  <si>
-    <t>Central Hardwoods (BCR 24)</t>
-  </si>
-  <si>
-    <t>West Gulf Coastal Plain/Ouachitas (BCR 25)</t>
-  </si>
-  <si>
-    <t>Mississippi Alluvial Valley (BCR 26)</t>
-  </si>
-  <si>
-    <t>Southeastern Coastal Plain (BCR 27)</t>
-  </si>
-  <si>
-    <t>Appalachian Mountains (BCR 28)</t>
-  </si>
-  <si>
-    <t>Piedmont (BCR 29)</t>
-  </si>
-  <si>
-    <t>New England/MidAtlantic Coasts (BCR 30)</t>
-  </si>
-  <si>
-    <t>Peninsular Florida (BCR 31)</t>
-  </si>
-  <si>
-    <t>Coastal California (BCR 32)</t>
-  </si>
-  <si>
-    <t>Sonoran and Mojave Deserts (BCR 33)</t>
-  </si>
-  <si>
-    <t>Sierra Madre Occidental (BCR 34)</t>
-  </si>
-  <si>
-    <t>Chihuahuan Desert (BCR 35)</t>
-  </si>
-  <si>
-    <t>Tamaulipan Brushlands (BCR 36)</t>
-  </si>
-  <si>
-    <t>Gulf Coastal Prairie (BCR 37)</t>
-  </si>
-  <si>
     <t>Seaducks</t>
   </si>
   <si>
@@ -847,115 +736,226 @@
     <t>zacatecas</t>
   </si>
   <si>
-    <t>aleutian/bering-sea-islands-(bcr-1)</t>
-  </si>
-  <si>
-    <t>western-alaska-(bcr-2)</t>
-  </si>
-  <si>
-    <t>arctic-plains-and-mountains-(bcr-3)</t>
-  </si>
-  <si>
-    <t>northwestern-interior-forest(bcr-4)</t>
-  </si>
-  <si>
-    <t>northern-pacific-rainforest-(bcr-5)</t>
-  </si>
-  <si>
-    <t>boreal-taiga-plains-(bcr-6)</t>
-  </si>
-  <si>
-    <t>taiga-shield-and-hudson-plain-(bcr-7)</t>
-  </si>
-  <si>
-    <t>boreal-softwood-shield-(bcr-8)</t>
-  </si>
-  <si>
-    <t>great-basin-(bcr-9)</t>
-  </si>
-  <si>
-    <t>northern-rockies-(bcr-10)</t>
-  </si>
-  <si>
-    <t>prairie-potholes-(bcr-11)</t>
-  </si>
-  <si>
-    <t>boreal-hardwood-transition-(bcr-12)</t>
-  </si>
-  <si>
-    <t>lower-great-lakes/st.lawrence-plain-(bcr-13)</t>
-  </si>
-  <si>
-    <t>atlantic-northern-forests-(bcr-14)</t>
-  </si>
-  <si>
-    <t>sierra-nevada-(bcr-15)</t>
-  </si>
-  <si>
-    <t>southern-rockies-colorado-plateau-(bcr-16)</t>
-  </si>
-  <si>
-    <t>badlands-and-prairies-(bcr-17)</t>
-  </si>
-  <si>
-    <t>shortgrass-prairie-(bcr-18)</t>
-  </si>
-  <si>
-    <t>central-mixed-grass-prairie-(bcr-19)</t>
-  </si>
-  <si>
-    <t>edwards-plateau-(bcr-20)</t>
-  </si>
-  <si>
-    <t>oaks-and-prairies-(bcr-21)</t>
-  </si>
-  <si>
-    <t>eastern-tallgrass-prairie-(bcr-22)</t>
-  </si>
-  <si>
-    <t>prairie-hardwood-transition-(bcr-23)</t>
-  </si>
-  <si>
-    <t>central-hardwoods-(bcr-24)</t>
-  </si>
-  <si>
-    <t>west-gulf-coastal-plain/ouachitas-(bcr-25)</t>
-  </si>
-  <si>
-    <t>mississippi-alluvial-valley-(bcr-26)</t>
-  </si>
-  <si>
-    <t>southeastern-coastal-plain-(bcr-27)</t>
-  </si>
-  <si>
-    <t>appalachian-mountains-(bcr-28)</t>
-  </si>
-  <si>
-    <t>piedmont-(bcr-29)</t>
-  </si>
-  <si>
-    <t>new-england/midatlantic-coasts-(bcr-30)</t>
-  </si>
-  <si>
-    <t>peninsular-florida-(bcr-31)</t>
-  </si>
-  <si>
-    <t>coastal-california-(bcr-32)</t>
-  </si>
-  <si>
-    <t>sonoran-and-mojave-deserts-(bcr-33)</t>
-  </si>
-  <si>
-    <t>sierra-madre-occidental-(bcr-34)</t>
-  </si>
-  <si>
-    <t>chihuahuan-desert-(bcr-35)</t>
-  </si>
-  <si>
-    <t>tamaulipan-brushlands-(bcr-36)</t>
-  </si>
-  <si>
-    <t>gulf-coastal-prairie-(bcr-37)</t>
+    <t>BCR 5-Northern Pacific Rainforest</t>
+  </si>
+  <si>
+    <t>BCR 6-Boreal Taiga Plains</t>
+  </si>
+  <si>
+    <t>BCR 1-Aleutian/Bering Sea Islands</t>
+  </si>
+  <si>
+    <t>BCR 2-Western Alaska</t>
+  </si>
+  <si>
+    <t>BCR 3-Arctic Plains and Mountains</t>
+  </si>
+  <si>
+    <t>BCR 7-Taiga Shield and Hudson Plain</t>
+  </si>
+  <si>
+    <t>BCR 8-Boreal Softwood Shield</t>
+  </si>
+  <si>
+    <t>BCR 9-Great Basin</t>
+  </si>
+  <si>
+    <t>BCR 10-Northern Rockies</t>
+  </si>
+  <si>
+    <t>BCR 11-Prairie Potholes</t>
+  </si>
+  <si>
+    <t>BCR 12-Boreal Hardwood Transition</t>
+  </si>
+  <si>
+    <t>BCR 13-Lower Great Lakes/St.Lawrence Plain</t>
+  </si>
+  <si>
+    <t>BCR 14-Atlantic Northern Forests</t>
+  </si>
+  <si>
+    <t>BCR 15-Sierra Nevada</t>
+  </si>
+  <si>
+    <t>BCR 16-Southern Rockies Colorado Plateau</t>
+  </si>
+  <si>
+    <t>BCR 17-Badlands and Prairies</t>
+  </si>
+  <si>
+    <t>BCR 18-Shortgrass Prairie</t>
+  </si>
+  <si>
+    <t>BCR 19-Central Mixed Grass Prairie</t>
+  </si>
+  <si>
+    <t>BCR 20-Edwards Plateau</t>
+  </si>
+  <si>
+    <t>BCR 21-Oaks and Prairies</t>
+  </si>
+  <si>
+    <t>BCR 22-Eastern Tallgrass Prairie</t>
+  </si>
+  <si>
+    <t>BCR 23-Prairie Hardwood Transition</t>
+  </si>
+  <si>
+    <t>BCR 24-Central Hardwoods</t>
+  </si>
+  <si>
+    <t>BCR 25-West Gulf Coastal Plain/Ouachitas</t>
+  </si>
+  <si>
+    <t>BCR 26-Mississippi Alluvial Valley</t>
+  </si>
+  <si>
+    <t>BCR 27-Southeastern Coastal Plain</t>
+  </si>
+  <si>
+    <t>BCR 28-Appalachian Mountains</t>
+  </si>
+  <si>
+    <t>BCR 29-Piedmont</t>
+  </si>
+  <si>
+    <t>BCR 30-New England/MidAtlantic Coasts</t>
+  </si>
+  <si>
+    <t>BCR 31-Peninsular Florida</t>
+  </si>
+  <si>
+    <t>BCR 32-Coastal California</t>
+  </si>
+  <si>
+    <t>BCR 33-Sonoran and Mojave Deserts</t>
+  </si>
+  <si>
+    <t>BCR 34-Sierra Madre Occidental</t>
+  </si>
+  <si>
+    <t>BCR 35-Chihuahuan Desert</t>
+  </si>
+  <si>
+    <t>BCR 36-Tamaulipan Brushlands</t>
+  </si>
+  <si>
+    <t>BCR 37-Gulf Coastal Prairie</t>
+  </si>
+  <si>
+    <t>BCR 4-Northwestern Interior Forest</t>
+  </si>
+  <si>
+    <t>BCR-1-Aleutian/Bering-Sea-Islands</t>
+  </si>
+  <si>
+    <t>BCR-2-Western-Alaska</t>
+  </si>
+  <si>
+    <t>BCR-3-Arctic-Plains-and-Mountains</t>
+  </si>
+  <si>
+    <t>BCR-4-Northwestern-Interior-Forest</t>
+  </si>
+  <si>
+    <t>BCR-5-Northern-Pacific-Rainforest</t>
+  </si>
+  <si>
+    <t>BCR-6-Boreal-Taiga-Plains</t>
+  </si>
+  <si>
+    <t>BCR-7-Taiga-Shield-and-Hudson-Plain</t>
+  </si>
+  <si>
+    <t>BCR-8-Boreal-Softwood-Shield</t>
+  </si>
+  <si>
+    <t>BCR-9-Great-Basin</t>
+  </si>
+  <si>
+    <t>BCR-10-Northern-Rockies</t>
+  </si>
+  <si>
+    <t>BCR-11-Prairie-Potholes</t>
+  </si>
+  <si>
+    <t>BCR-12-Boreal-Hardwood-Transition</t>
+  </si>
+  <si>
+    <t>BCR-13-Lower-Great-Lakes/St.Lawrence-Plain</t>
+  </si>
+  <si>
+    <t>BCR-14-Atlantic-Northern-Forests</t>
+  </si>
+  <si>
+    <t>BCR-15-Sierra-Nevada</t>
+  </si>
+  <si>
+    <t>BCR-16-Southern-Rockies-Colorado-Plateau</t>
+  </si>
+  <si>
+    <t>BCR-17-Badlands-and-Prairies</t>
+  </si>
+  <si>
+    <t>BCR-18-Shortgrass-Prairie</t>
+  </si>
+  <si>
+    <t>BCR-19-Central-Mixed-Grass-Prairie</t>
+  </si>
+  <si>
+    <t>BCR-20-Edwards-Plateau</t>
+  </si>
+  <si>
+    <t>BCR-21-Oaks-and-Prairies</t>
+  </si>
+  <si>
+    <t>BCR-22-Eastern-Tallgrass-Prairie</t>
+  </si>
+  <si>
+    <t>BCR-23-Prairie-Hardwood-Transition</t>
+  </si>
+  <si>
+    <t>BCR-24-Central-Hardwoods</t>
+  </si>
+  <si>
+    <t>BCR-25-West-Gulf-Coastal-Plain/Ouachitas</t>
+  </si>
+  <si>
+    <t>BCR-26-Mississippi-Alluvial-Valley</t>
+  </si>
+  <si>
+    <t>BCR-27-Southeastern-Coastal-Plain</t>
+  </si>
+  <si>
+    <t>BCR-28-Appalachian-Mountains</t>
+  </si>
+  <si>
+    <t>BCR-29-Piedmont</t>
+  </si>
+  <si>
+    <t>BCR-30-New-England/MidAtlantic-Coasts</t>
+  </si>
+  <si>
+    <t>BCR-31-Peninsular-Florida</t>
+  </si>
+  <si>
+    <t>BCR-32-Coastal-California</t>
+  </si>
+  <si>
+    <t>BCR-33-Sonoran-and-Mojave-Deserts</t>
+  </si>
+  <si>
+    <t>BCR-34-Sierra-Madre-Occidental</t>
+  </si>
+  <si>
+    <t>BCR-35-Chihuahuan-Desert</t>
+  </si>
+  <si>
+    <t>BCR-36-Tamaulipan-Brushlands</t>
+  </si>
+  <si>
+    <t>BCR-37-Gulf-Coastal-Prairie</t>
   </si>
 </sst>
 </file>
@@ -1783,7 +1783,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>156</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1791,10 +1791,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>155</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
-        <v>157</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1805,7 +1805,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>158</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1816,7 +1816,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>159</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1827,7 +1827,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>160</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1838,7 +1838,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>161</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1849,7 +1849,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>162</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1860,7 +1860,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>163</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1871,7 +1871,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>164</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1882,7 +1882,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>165</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1893,7 +1893,7 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>166</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1904,7 +1904,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>167</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1915,7 +1915,7 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>168</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1926,7 +1926,7 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>169</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1937,7 +1937,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>174</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1948,7 +1948,7 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>175</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1959,7 +1959,7 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>176</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1970,7 +1970,7 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>170</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1981,7 +1981,7 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>171</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1992,7 +1992,7 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>172</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2003,7 +2003,7 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>173</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2014,7 +2014,7 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>177</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2026,8 +2026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="C139" sqref="C139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2044,7 +2044,7 @@
         <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>178</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2055,7 +2055,7 @@
         <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>179</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2066,7 +2066,7 @@
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>180</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2077,7 +2077,7 @@
         <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>181</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2088,7 +2088,7 @@
         <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>182</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2099,7 +2099,7 @@
         <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>183</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2110,7 +2110,7 @@
         <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>184</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2121,7 +2121,7 @@
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>185</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2132,7 +2132,7 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>186</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2143,7 +2143,7 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>187</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2154,7 +2154,7 @@
         <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>188</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2165,7 +2165,7 @@
         <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>189</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2176,7 +2176,7 @@
         <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>190</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2187,7 +2187,7 @@
         <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>191</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2198,7 +2198,7 @@
         <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>192</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2209,7 +2209,7 @@
         <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>193</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2220,7 +2220,7 @@
         <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>194</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2231,7 +2231,7 @@
         <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>195</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2242,7 +2242,7 @@
         <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>196</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2253,7 +2253,7 @@
         <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>197</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2264,7 +2264,7 @@
         <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>198</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2275,7 +2275,7 @@
         <v>42</v>
       </c>
       <c r="C22" t="s">
-        <v>199</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2286,7 +2286,7 @@
         <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>200</v>
+        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2297,7 +2297,7 @@
         <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>201</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2308,7 +2308,7 @@
         <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -2319,7 +2319,7 @@
         <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>203</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2330,7 +2330,7 @@
         <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>204</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -2341,7 +2341,7 @@
         <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>205</v>
+        <v>168</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -2352,7 +2352,7 @@
         <v>49</v>
       </c>
       <c r="C29" t="s">
-        <v>206</v>
+        <v>169</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -2363,7 +2363,7 @@
         <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>207</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2374,7 +2374,7 @@
         <v>51</v>
       </c>
       <c r="C31" t="s">
-        <v>208</v>
+        <v>171</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2385,7 +2385,7 @@
         <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>209</v>
+        <v>172</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -2396,7 +2396,7 @@
         <v>53</v>
       </c>
       <c r="C33" t="s">
-        <v>210</v>
+        <v>173</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2407,7 +2407,7 @@
         <v>54</v>
       </c>
       <c r="C34" t="s">
-        <v>211</v>
+        <v>174</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -2418,7 +2418,7 @@
         <v>55</v>
       </c>
       <c r="C35" t="s">
-        <v>212</v>
+        <v>175</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -2429,7 +2429,7 @@
         <v>56</v>
       </c>
       <c r="C36" t="s">
-        <v>213</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -2440,7 +2440,7 @@
         <v>57</v>
       </c>
       <c r="C37" t="s">
-        <v>214</v>
+        <v>177</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -2451,7 +2451,7 @@
         <v>58</v>
       </c>
       <c r="C38" t="s">
-        <v>215</v>
+        <v>178</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -2462,7 +2462,7 @@
         <v>59</v>
       </c>
       <c r="C39" t="s">
-        <v>216</v>
+        <v>179</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -2473,7 +2473,7 @@
         <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>217</v>
+        <v>180</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -2484,7 +2484,7 @@
         <v>61</v>
       </c>
       <c r="C41" t="s">
-        <v>218</v>
+        <v>181</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -2495,7 +2495,7 @@
         <v>62</v>
       </c>
       <c r="C42" t="s">
-        <v>219</v>
+        <v>182</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -2506,7 +2506,7 @@
         <v>63</v>
       </c>
       <c r="C43" t="s">
-        <v>220</v>
+        <v>183</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -2517,7 +2517,7 @@
         <v>64</v>
       </c>
       <c r="C44" t="s">
-        <v>221</v>
+        <v>184</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -2528,7 +2528,7 @@
         <v>65</v>
       </c>
       <c r="C45" t="s">
-        <v>222</v>
+        <v>185</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -2539,7 +2539,7 @@
         <v>66</v>
       </c>
       <c r="C46" t="s">
-        <v>223</v>
+        <v>186</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -2550,7 +2550,7 @@
         <v>67</v>
       </c>
       <c r="C47" t="s">
-        <v>224</v>
+        <v>187</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -2561,7 +2561,7 @@
         <v>68</v>
       </c>
       <c r="C48" t="s">
-        <v>225</v>
+        <v>188</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -2572,7 +2572,7 @@
         <v>69</v>
       </c>
       <c r="C49" t="s">
-        <v>226</v>
+        <v>189</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -2583,7 +2583,7 @@
         <v>70</v>
       </c>
       <c r="C50" t="s">
-        <v>227</v>
+        <v>190</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -2594,7 +2594,7 @@
         <v>71</v>
       </c>
       <c r="C51" t="s">
-        <v>228</v>
+        <v>191</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -2605,7 +2605,7 @@
         <v>72</v>
       </c>
       <c r="C52" t="s">
-        <v>229</v>
+        <v>192</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -2616,7 +2616,7 @@
         <v>73</v>
       </c>
       <c r="C53" t="s">
-        <v>230</v>
+        <v>193</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -2627,7 +2627,7 @@
         <v>74</v>
       </c>
       <c r="C54" t="s">
-        <v>231</v>
+        <v>194</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -2638,7 +2638,7 @@
         <v>75</v>
       </c>
       <c r="C55" t="s">
-        <v>232</v>
+        <v>195</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -2649,7 +2649,7 @@
         <v>76</v>
       </c>
       <c r="C56" t="s">
-        <v>233</v>
+        <v>196</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -2660,7 +2660,7 @@
         <v>77</v>
       </c>
       <c r="C57" t="s">
-        <v>234</v>
+        <v>197</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -2671,7 +2671,7 @@
         <v>78</v>
       </c>
       <c r="C58" t="s">
-        <v>235</v>
+        <v>198</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -2682,7 +2682,7 @@
         <v>79</v>
       </c>
       <c r="C59" t="s">
-        <v>236</v>
+        <v>199</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -2693,7 +2693,7 @@
         <v>80</v>
       </c>
       <c r="C60" t="s">
-        <v>237</v>
+        <v>200</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -2704,7 +2704,7 @@
         <v>81</v>
       </c>
       <c r="C61" t="s">
-        <v>238</v>
+        <v>201</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -2715,7 +2715,7 @@
         <v>82</v>
       </c>
       <c r="C62" t="s">
-        <v>239</v>
+        <v>202</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -2726,7 +2726,7 @@
         <v>83</v>
       </c>
       <c r="C63" t="s">
-        <v>240</v>
+        <v>203</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -2737,7 +2737,7 @@
         <v>84</v>
       </c>
       <c r="C64" t="s">
-        <v>241</v>
+        <v>204</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -2748,7 +2748,7 @@
         <v>85</v>
       </c>
       <c r="C65" t="s">
-        <v>242</v>
+        <v>205</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -2759,7 +2759,7 @@
         <v>86</v>
       </c>
       <c r="C66" t="s">
-        <v>243</v>
+        <v>206</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -2770,7 +2770,7 @@
         <v>87</v>
       </c>
       <c r="C67" t="s">
-        <v>244</v>
+        <v>207</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -2781,7 +2781,7 @@
         <v>88</v>
       </c>
       <c r="C68" t="s">
-        <v>245</v>
+        <v>208</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -2792,7 +2792,7 @@
         <v>89</v>
       </c>
       <c r="C69" t="s">
-        <v>246</v>
+        <v>209</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -2803,7 +2803,7 @@
         <v>90</v>
       </c>
       <c r="C70" t="s">
-        <v>247</v>
+        <v>210</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -2814,7 +2814,7 @@
         <v>91</v>
       </c>
       <c r="C71" t="s">
-        <v>248</v>
+        <v>211</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -2825,7 +2825,7 @@
         <v>92</v>
       </c>
       <c r="C72" t="s">
-        <v>249</v>
+        <v>212</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -2836,7 +2836,7 @@
         <v>93</v>
       </c>
       <c r="C73" t="s">
-        <v>250</v>
+        <v>213</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -2847,7 +2847,7 @@
         <v>94</v>
       </c>
       <c r="C74" t="s">
-        <v>251</v>
+        <v>214</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -2858,7 +2858,7 @@
         <v>95</v>
       </c>
       <c r="C75" t="s">
-        <v>252</v>
+        <v>215</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -2869,7 +2869,7 @@
         <v>96</v>
       </c>
       <c r="C76" t="s">
-        <v>253</v>
+        <v>216</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -2880,7 +2880,7 @@
         <v>97</v>
       </c>
       <c r="C77" t="s">
-        <v>254</v>
+        <v>217</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -2891,7 +2891,7 @@
         <v>98</v>
       </c>
       <c r="C78" t="s">
-        <v>255</v>
+        <v>218</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -2902,7 +2902,7 @@
         <v>99</v>
       </c>
       <c r="C79" t="s">
-        <v>256</v>
+        <v>219</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -2913,7 +2913,7 @@
         <v>100</v>
       </c>
       <c r="C80" t="s">
-        <v>257</v>
+        <v>220</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -2924,7 +2924,7 @@
         <v>101</v>
       </c>
       <c r="C81" t="s">
-        <v>258</v>
+        <v>221</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -2935,7 +2935,7 @@
         <v>102</v>
       </c>
       <c r="C82" t="s">
-        <v>259</v>
+        <v>222</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -2946,7 +2946,7 @@
         <v>103</v>
       </c>
       <c r="C83" t="s">
-        <v>260</v>
+        <v>223</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -2957,7 +2957,7 @@
         <v>104</v>
       </c>
       <c r="C84" t="s">
-        <v>261</v>
+        <v>224</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -2968,7 +2968,7 @@
         <v>105</v>
       </c>
       <c r="C85" t="s">
-        <v>262</v>
+        <v>225</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -2979,7 +2979,7 @@
         <v>106</v>
       </c>
       <c r="C86" t="s">
-        <v>263</v>
+        <v>226</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -2990,7 +2990,7 @@
         <v>107</v>
       </c>
       <c r="C87" t="s">
-        <v>264</v>
+        <v>227</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -3001,7 +3001,7 @@
         <v>108</v>
       </c>
       <c r="C88" t="s">
-        <v>265</v>
+        <v>228</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -3012,7 +3012,7 @@
         <v>109</v>
       </c>
       <c r="C89" t="s">
-        <v>266</v>
+        <v>229</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -3023,7 +3023,7 @@
         <v>110</v>
       </c>
       <c r="C90" t="s">
-        <v>267</v>
+        <v>230</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -3034,7 +3034,7 @@
         <v>111</v>
       </c>
       <c r="C91" t="s">
-        <v>268</v>
+        <v>231</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -3045,7 +3045,7 @@
         <v>112</v>
       </c>
       <c r="C92" t="s">
-        <v>269</v>
+        <v>232</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -3056,7 +3056,7 @@
         <v>113</v>
       </c>
       <c r="C93" t="s">
-        <v>270</v>
+        <v>233</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -3067,7 +3067,7 @@
         <v>114</v>
       </c>
       <c r="C94" t="s">
-        <v>271</v>
+        <v>234</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -3078,7 +3078,7 @@
         <v>115</v>
       </c>
       <c r="C95" t="s">
-        <v>272</v>
+        <v>235</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -3089,7 +3089,7 @@
         <v>116</v>
       </c>
       <c r="C96" t="s">
-        <v>273</v>
+        <v>236</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -3100,7 +3100,7 @@
         <v>117</v>
       </c>
       <c r="C97" t="s">
-        <v>274</v>
+        <v>237</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -3108,7 +3108,7 @@
         <v>98</v>
       </c>
       <c r="B98" t="s">
-        <v>118</v>
+        <v>240</v>
       </c>
       <c r="C98" t="s">
         <v>275</v>
@@ -3119,7 +3119,7 @@
         <v>99</v>
       </c>
       <c r="B99" t="s">
-        <v>119</v>
+        <v>241</v>
       </c>
       <c r="C99" t="s">
         <v>276</v>
@@ -3130,7 +3130,7 @@
         <v>100</v>
       </c>
       <c r="B100" t="s">
-        <v>120</v>
+        <v>242</v>
       </c>
       <c r="C100" t="s">
         <v>277</v>
@@ -3141,7 +3141,7 @@
         <v>101</v>
       </c>
       <c r="B101" t="s">
-        <v>121</v>
+        <v>274</v>
       </c>
       <c r="C101" t="s">
         <v>278</v>
@@ -3152,7 +3152,7 @@
         <v>102</v>
       </c>
       <c r="B102" t="s">
-        <v>122</v>
+        <v>238</v>
       </c>
       <c r="C102" t="s">
         <v>279</v>
@@ -3163,7 +3163,7 @@
         <v>103</v>
       </c>
       <c r="B103" t="s">
-        <v>123</v>
+        <v>239</v>
       </c>
       <c r="C103" t="s">
         <v>280</v>
@@ -3174,7 +3174,7 @@
         <v>104</v>
       </c>
       <c r="B104" t="s">
-        <v>124</v>
+        <v>243</v>
       </c>
       <c r="C104" t="s">
         <v>281</v>
@@ -3185,7 +3185,7 @@
         <v>105</v>
       </c>
       <c r="B105" t="s">
-        <v>125</v>
+        <v>244</v>
       </c>
       <c r="C105" t="s">
         <v>282</v>
@@ -3196,7 +3196,7 @@
         <v>106</v>
       </c>
       <c r="B106" t="s">
-        <v>126</v>
+        <v>245</v>
       </c>
       <c r="C106" t="s">
         <v>283</v>
@@ -3207,7 +3207,7 @@
         <v>107</v>
       </c>
       <c r="B107" t="s">
-        <v>127</v>
+        <v>246</v>
       </c>
       <c r="C107" t="s">
         <v>284</v>
@@ -3218,7 +3218,7 @@
         <v>108</v>
       </c>
       <c r="B108" t="s">
-        <v>128</v>
+        <v>247</v>
       </c>
       <c r="C108" t="s">
         <v>285</v>
@@ -3229,7 +3229,7 @@
         <v>109</v>
       </c>
       <c r="B109" t="s">
-        <v>129</v>
+        <v>248</v>
       </c>
       <c r="C109" t="s">
         <v>286</v>
@@ -3240,7 +3240,7 @@
         <v>110</v>
       </c>
       <c r="B110" t="s">
-        <v>130</v>
+        <v>249</v>
       </c>
       <c r="C110" t="s">
         <v>287</v>
@@ -3251,7 +3251,7 @@
         <v>111</v>
       </c>
       <c r="B111" t="s">
-        <v>131</v>
+        <v>250</v>
       </c>
       <c r="C111" t="s">
         <v>288</v>
@@ -3262,7 +3262,7 @@
         <v>112</v>
       </c>
       <c r="B112" t="s">
-        <v>132</v>
+        <v>251</v>
       </c>
       <c r="C112" t="s">
         <v>289</v>
@@ -3273,7 +3273,7 @@
         <v>113</v>
       </c>
       <c r="B113" t="s">
-        <v>133</v>
+        <v>252</v>
       </c>
       <c r="C113" t="s">
         <v>290</v>
@@ -3284,7 +3284,7 @@
         <v>114</v>
       </c>
       <c r="B114" t="s">
-        <v>134</v>
+        <v>253</v>
       </c>
       <c r="C114" t="s">
         <v>291</v>
@@ -3295,7 +3295,7 @@
         <v>115</v>
       </c>
       <c r="B115" t="s">
-        <v>135</v>
+        <v>254</v>
       </c>
       <c r="C115" t="s">
         <v>292</v>
@@ -3306,7 +3306,7 @@
         <v>116</v>
       </c>
       <c r="B116" t="s">
-        <v>136</v>
+        <v>255</v>
       </c>
       <c r="C116" t="s">
         <v>293</v>
@@ -3317,7 +3317,7 @@
         <v>117</v>
       </c>
       <c r="B117" t="s">
-        <v>137</v>
+        <v>256</v>
       </c>
       <c r="C117" t="s">
         <v>294</v>
@@ -3328,7 +3328,7 @@
         <v>118</v>
       </c>
       <c r="B118" t="s">
-        <v>138</v>
+        <v>257</v>
       </c>
       <c r="C118" t="s">
         <v>295</v>
@@ -3339,7 +3339,7 @@
         <v>119</v>
       </c>
       <c r="B119" t="s">
-        <v>139</v>
+        <v>258</v>
       </c>
       <c r="C119" t="s">
         <v>296</v>
@@ -3350,7 +3350,7 @@
         <v>120</v>
       </c>
       <c r="B120" t="s">
-        <v>140</v>
+        <v>259</v>
       </c>
       <c r="C120" t="s">
         <v>297</v>
@@ -3361,7 +3361,7 @@
         <v>121</v>
       </c>
       <c r="B121" t="s">
-        <v>141</v>
+        <v>260</v>
       </c>
       <c r="C121" t="s">
         <v>298</v>
@@ -3372,7 +3372,7 @@
         <v>122</v>
       </c>
       <c r="B122" t="s">
-        <v>142</v>
+        <v>261</v>
       </c>
       <c r="C122" t="s">
         <v>299</v>
@@ -3383,7 +3383,7 @@
         <v>123</v>
       </c>
       <c r="B123" t="s">
-        <v>143</v>
+        <v>262</v>
       </c>
       <c r="C123" t="s">
         <v>300</v>
@@ -3394,7 +3394,7 @@
         <v>124</v>
       </c>
       <c r="B124" t="s">
-        <v>144</v>
+        <v>263</v>
       </c>
       <c r="C124" t="s">
         <v>301</v>
@@ -3405,7 +3405,7 @@
         <v>125</v>
       </c>
       <c r="B125" t="s">
-        <v>145</v>
+        <v>264</v>
       </c>
       <c r="C125" t="s">
         <v>302</v>
@@ -3416,7 +3416,7 @@
         <v>126</v>
       </c>
       <c r="B126" t="s">
-        <v>146</v>
+        <v>265</v>
       </c>
       <c r="C126" t="s">
         <v>303</v>
@@ -3427,7 +3427,7 @@
         <v>127</v>
       </c>
       <c r="B127" t="s">
-        <v>147</v>
+        <v>266</v>
       </c>
       <c r="C127" t="s">
         <v>304</v>
@@ -3438,7 +3438,7 @@
         <v>128</v>
       </c>
       <c r="B128" t="s">
-        <v>148</v>
+        <v>267</v>
       </c>
       <c r="C128" t="s">
         <v>305</v>
@@ -3449,7 +3449,7 @@
         <v>129</v>
       </c>
       <c r="B129" t="s">
-        <v>149</v>
+        <v>268</v>
       </c>
       <c r="C129" t="s">
         <v>306</v>
@@ -3460,7 +3460,7 @@
         <v>130</v>
       </c>
       <c r="B130" t="s">
-        <v>150</v>
+        <v>269</v>
       </c>
       <c r="C130" t="s">
         <v>307</v>
@@ -3471,7 +3471,7 @@
         <v>131</v>
       </c>
       <c r="B131" t="s">
-        <v>151</v>
+        <v>270</v>
       </c>
       <c r="C131" t="s">
         <v>308</v>
@@ -3482,7 +3482,7 @@
         <v>132</v>
       </c>
       <c r="B132" t="s">
-        <v>152</v>
+        <v>271</v>
       </c>
       <c r="C132" t="s">
         <v>309</v>
@@ -3493,7 +3493,7 @@
         <v>133</v>
       </c>
       <c r="B133" t="s">
-        <v>153</v>
+        <v>272</v>
       </c>
       <c r="C133" t="s">
         <v>310</v>
@@ -3504,7 +3504,7 @@
         <v>134</v>
       </c>
       <c r="B134" t="s">
-        <v>154</v>
+        <v>273</v>
       </c>
       <c r="C134" t="s">
         <v>311</v>

</xml_diff>